<commit_message>
First version of ChargingController
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3838EA-7993-4E45-ABC6-1702423AAB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED25F9-DBA0-44C8-B9B7-6AA8C15D1135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>FromGrid%</t>
+  </si>
+  <si>
+    <t>CurrentInside</t>
+  </si>
+  <si>
+    <t>CurrentOutside</t>
   </si>
 </sst>
 </file>
@@ -107,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -404,9 +411,10 @@
     <col min="6" max="6" width="13.06640625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.06640625" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -437,8 +445,14 @@
       <c r="J1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,7 +463,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>-4500</v>
+        <v>-4500000</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -467,10 +481,18 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4500000</v>
+      </c>
+      <c r="K2" s="1">
+        <f>I2/3/230*1000</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <f>J2/3/230</f>
+        <v>6521.739130434783</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -481,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>-4500</v>
+        <v>-4500000</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -496,13 +518,21 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K3" s="1">
+        <f>I3/3/230</f>
+        <v>6521.739130434783</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="K3:L16" si="0">J3/3/230*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -513,13 +543,13 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>-4500</v>
+        <v>-4500000</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -531,10 +561,18 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+        <v>9000000</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <f>J4/3/230</f>
+        <v>13043.478260869566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -545,10 +583,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>-4500</v>
+        <v>-4500000</v>
       </c>
       <c r="E5">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -560,13 +598,21 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>9000</v>
+        <v>9000000</v>
       </c>
       <c r="J5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K5" s="1">
+        <f>I5/3/230</f>
+        <v>13043.478260869566</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -577,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>-4500</v>
+        <v>-4500000</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -592,13 +638,21 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K6" s="1">
+        <f>I6/3/230</f>
+        <v>6521.739130434783</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -609,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <v>-4500</v>
+        <v>-4500000</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -627,10 +681,18 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4500000</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f>J7/3/230</f>
+        <v>6521.739130434783</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -641,10 +703,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>-4000</v>
+        <v>-4000000</v>
       </c>
       <c r="E8">
-        <v>4000</v>
+        <v>4000000</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -656,13 +718,21 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>8000</v>
+        <v>8000000</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K8" s="1">
+        <f>I8/3/230</f>
+        <v>11594.202898550724</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -673,13 +743,13 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>-4000</v>
+        <v>-4000000</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>4000</v>
+        <v>4000000</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>
@@ -691,10 +761,18 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+        <v>8000000</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <f>J9/3/230</f>
+        <v>11594.202898550724</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -705,13 +783,13 @@
         <v>1</v>
       </c>
       <c r="D10">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>8000</v>
+        <v>8000000</v>
       </c>
       <c r="G10" t="s">
         <v>9</v>
@@ -723,10 +801,18 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+        <v>6000000</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <f>J10/3/230</f>
+        <v>8695.652173913044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -737,13 +823,13 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
@@ -757,8 +843,16 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -769,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E12">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -789,8 +883,16 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -801,13 +903,13 @@
         <v>1</v>
       </c>
       <c r="D13">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
@@ -819,11 +921,19 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <f>230*6*3</f>
-        <v>4140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+        <f>230*6*3*1000</f>
+        <v>4140000</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f>J13/3/230</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -834,10 +944,10 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E14">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -849,14 +959,22 @@
         <v>50</v>
       </c>
       <c r="I14">
-        <f>230*6*3</f>
-        <v>4140</v>
+        <f>230*6*3*1000</f>
+        <v>4140000</v>
       </c>
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K14" s="1">
+        <f>I14/3/230</f>
+        <v>6000</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -867,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>-9000</v>
+        <v>-9000000</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -882,13 +1000,21 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>4500</v>
+        <v>4500000</v>
       </c>
       <c r="J15">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+        <v>4500000</v>
+      </c>
+      <c r="K15" s="1">
+        <f>I15/3/230</f>
+        <v>6521.739130434783</v>
+      </c>
+      <c r="L15" s="1">
+        <f>J15/3/230</f>
+        <v>6521.739130434783</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -899,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>2000</v>
+        <v>2000000</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -914,10 +1040,18 @@
         <v>100</v>
       </c>
       <c r="I16">
-        <f>230*6*3</f>
-        <v>4140</v>
+        <f>230*6*3*1000</f>
+        <v>4140000</v>
       </c>
       <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f>I16/3/230</f>
+        <v>6000</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Includeing battery level in charging decision
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED25F9-DBA0-44C8-B9B7-6AA8C15D1135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E874F59-8396-438F-B1D0-7DABDB21D98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>CurrentOutside</t>
+  </si>
+  <si>
+    <t>BatteryLevel</t>
+  </si>
+  <si>
+    <t>BatteryMinLevel</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -409,12 +415,12 @@
     <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.06640625" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13.06640625" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -440,19 +446,25 @@
         <v>11</v>
       </c>
       <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,18 +493,24 @@
         <v>0</v>
       </c>
       <c r="J2">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>4500000</v>
       </c>
-      <c r="K2" s="1">
-        <f>I2/3/230*1000</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <f>J2/3/230</f>
+      <c r="M2" s="1">
+        <f>K2/3/230*1000</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <f>L2/3/230</f>
         <v>6521.739130434783</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -518,21 +536,27 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>25</v>
+      </c>
+      <c r="K3">
         <v>4500000</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <f>I3/3/230</f>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <f>K3/3/230</f>
         <v>6521.739130434783</v>
       </c>
-      <c r="L3" s="1">
-        <f t="shared" ref="K3:L16" si="0">J3/3/230*1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N3" s="1">
+        <f t="shared" ref="M3:N16" si="0">L3/3/230*1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -561,18 +585,24 @@
         <v>0</v>
       </c>
       <c r="J4">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>9000000</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <f>J4/3/230</f>
+      <c r="M4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <f>L4/3/230</f>
         <v>13043.478260869566</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -598,21 +628,27 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>25</v>
+      </c>
+      <c r="K5">
         <v>9000000</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <f>I5/3/230</f>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <f>K5/3/230</f>
         <v>13043.478260869566</v>
       </c>
-      <c r="L5" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -638,21 +674,27 @@
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6">
         <v>4500000</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <f>I6/3/230</f>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <f>K6/3/230</f>
         <v>6521.739130434783</v>
       </c>
-      <c r="L6" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N6" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -681,18 +723,24 @@
         <v>0</v>
       </c>
       <c r="J7">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>4500000</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <f>J7/3/230</f>
+      <c r="M7" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <f>L7/3/230</f>
         <v>6521.739130434783</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -718,21 +766,27 @@
         <v>0</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>25</v>
+      </c>
+      <c r="K8">
         <v>8000000</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <f>I8/3/230</f>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <f>K8/3/230</f>
         <v>11594.202898550724</v>
       </c>
-      <c r="L8" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -761,18 +815,24 @@
         <v>0</v>
       </c>
       <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>8000000</v>
       </c>
-      <c r="K9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <f>J9/3/230</f>
+      <c r="M9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <f>L9/3/230</f>
         <v>11594.202898550724</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -801,18 +861,24 @@
         <v>0</v>
       </c>
       <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>6000000</v>
       </c>
-      <c r="K10" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L10" s="1">
-        <f>J10/3/230</f>
+      <c r="M10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10" s="1">
+        <f>L10/3/230</f>
         <v>8695.652173913044</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -841,18 +907,24 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -881,18 +953,24 @@
         <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -921,19 +999,25 @@
         <v>0</v>
       </c>
       <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <f>230*6*3*1000</f>
         <v>4140000</v>
       </c>
-      <c r="K13" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <f>J13/3/230</f>
+      <c r="M13" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <f>L13/3/230</f>
         <v>6000</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -959,22 +1043,28 @@
         <v>50</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>25</v>
+      </c>
+      <c r="K14">
         <f>230*6*3*1000</f>
         <v>4140000</v>
       </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
-        <f>I14/3/230</f>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <f>K14/3/230</f>
         <v>6000</v>
       </c>
-      <c r="L14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="N14" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1000,21 +1090,27 @@
         <v>0</v>
       </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>25</v>
+      </c>
+      <c r="K15">
         <v>4500000</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>4500000</v>
       </c>
-      <c r="K15" s="1">
-        <f>I15/3/230</f>
+      <c r="M15" s="1">
+        <f>K15/3/230</f>
         <v>6521.739130434783</v>
       </c>
-      <c r="L15" s="1">
-        <f>J15/3/230</f>
+      <c r="N15" s="1">
+        <f>L15/3/230</f>
         <v>6521.739130434783</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1040,19 +1136,70 @@
         <v>100</v>
       </c>
       <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="K16">
         <f>230*6*3*1000</f>
         <v>4140000</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <f>I16/3/230</f>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <f>K16/3/230</f>
         <v>6000</v>
       </c>
-      <c r="L16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="N16" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1000000</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>75</v>
+      </c>
+      <c r="J17">
+        <v>25</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>230*6*3*1000</f>
+        <v>4140000</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed to manually charge both stations when set to manual charging
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71090163-5C35-4481-8645-7B10732DAA91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7701280-1F04-4AB5-A730-5A2442B9ABFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1857,14 +1857,15 @@
         <v>6000</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <f>6000*230*3</f>
+        <v>4140000</v>
       </c>
       <c r="P25">
         <f>6000*230*3</f>
         <v>4140000</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="R25" s="1">
         <v>6000</v>

</xml_diff>

<commit_message>
Added enabling / disabling for charging
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696E7FD2-282F-4140-A658-C611EF2DD318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6622E073-3ED2-44F8-A282-D2E8305770B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Level</t>
+  </si>
+  <si>
+    <t>InsideEnabled</t>
+  </si>
+  <si>
+    <t>OutsideEnabled</t>
   </si>
 </sst>
 </file>
@@ -395,26 +401,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="6.06640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.9296875" customWidth="1"/>
-    <col min="8" max="8" width="11.53125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.06640625" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -428,34 +439,40 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -469,34 +486,40 @@
         <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>-4500</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>4500</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>100</v>
       </c>
-      <c r="K2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -510,34 +533,40 @@
         <v>1</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>-4500</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>4500</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>10</v>
       </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -551,34 +580,40 @@
         <v>1</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>-4500</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>4500</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>90</v>
       </c>
-      <c r="K4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -592,35 +627,41 @@
         <v>1</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>-9000</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>9000</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>10</v>
       </c>
-      <c r="K5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <f>F5-3800</f>
+      <c r="M5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>H5-3800</f>
         <v>5200</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -634,35 +675,41 @@
         <v>1</v>
       </c>
       <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>-4500</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>8000</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>-3500</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
       <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>10</v>
       </c>
-      <c r="K6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <f>F6-3800</f>
+      <c r="M6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>H6-3800</f>
         <v>4200</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -676,34 +723,40 @@
         <v>1</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
         <v>-2000</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>2000</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>10</v>
       </c>
-      <c r="K7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -717,34 +770,40 @@
         <v>1</v>
       </c>
       <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>-4500</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>4500</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8">
         <v>0</v>
       </c>
       <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>10</v>
       </c>
-      <c r="K8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
         <v>4500</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -758,34 +817,40 @@
         <v>1</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>-4500</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>4500</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>90</v>
       </c>
-      <c r="K9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
+      <c r="M9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>4500</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -799,34 +864,40 @@
         <v>1</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>-9000</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>9000</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>10</v>
       </c>
-      <c r="K10" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
         <v>9000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -840,34 +911,40 @@
         <v>1</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>-4500</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>8000</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>-3500</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
       <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>10</v>
       </c>
-      <c r="K11" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
+      <c r="M11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
         <v>8000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -881,34 +958,40 @@
         <v>1</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
         <v>-100</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>100</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
         <v>0</v>
       </c>
       <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>90</v>
       </c>
-      <c r="K12" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -922,34 +1005,40 @@
         <v>1</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>-2000</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>2000</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13">
         <v>0</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>10</v>
       </c>
-      <c r="K13" t="s">
-        <v>9</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -963,35 +1052,41 @@
         <v>1</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
         <v>-2000</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>2000</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
       <c r="I14">
         <v>0</v>
       </c>
       <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>50</v>
       </c>
-      <c r="K14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
+      <c r="M14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
         <f>230*6*3</f>
         <v>4140</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1005,34 +1100,40 @@
         <v>1</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
         <v>-4500</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>4500</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>10</v>
       </c>
-      <c r="K15" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
         <v>4140</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1046,34 +1147,40 @@
         <v>1</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
         <v>-4500</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>4500</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>90</v>
       </c>
-      <c r="K16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="M16">
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
         <v>4500</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1087,35 +1194,41 @@
         <v>1</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
         <v>-4500</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>8000</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>-3500</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
       <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>10</v>
       </c>
-      <c r="K17" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
+      <c r="M17" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
         <f>8000-3800</f>
         <v>4200</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1129,34 +1242,40 @@
         <v>1</v>
       </c>
       <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
         <v>-4500</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>8000</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>-3500</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
       <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>50</v>
       </c>
-      <c r="K18" t="s">
-        <v>9</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
+      <c r="M18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
         <v>8000</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1170,34 +1289,40 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>1000</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>3500</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
         <v>4500</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>50</v>
       </c>
-      <c r="K19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
+      <c r="M19" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
         <v>4140</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1211,14 +1336,14 @@
         <v>1</v>
       </c>
       <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
         <v>5000</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
       <c r="H20">
         <v>0</v>
       </c>
@@ -1226,19 +1351,25 @@
         <v>0</v>
       </c>
       <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
         <v>10</v>
       </c>
-      <c r="K20" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
         <v>4140</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1252,14 +1383,14 @@
         <v>1</v>
       </c>
       <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
         <v>5000</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
       <c r="H21">
         <v>0</v>
       </c>
@@ -1267,16 +1398,116 @@
         <v>0</v>
       </c>
       <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
         <v>10</v>
       </c>
-      <c r="K21" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
+      <c r="M21" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
         <v>8000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1300</v>
+      </c>
+      <c r="I22">
+        <v>-1000</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>98</v>
+      </c>
+      <c r="M22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>-9000</v>
+      </c>
+      <c r="H23">
+        <v>9000</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>98</v>
+      </c>
+      <c r="M23" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in charging controller
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6622E073-3ED2-44F8-A282-D2E8305770B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289C1B7E-BCFA-4114-8215-4AC2422EB7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>OutsideEnabled</t>
+  </si>
+  <si>
+    <t>Outside</t>
   </si>
 </sst>
 </file>
@@ -401,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1510,6 +1513,53 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>98</v>
+      </c>
+      <c r="M24" t="s">
+        <v>16</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more data to VW charging
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289C1B7E-BCFA-4114-8215-4AC2422EB7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62426A9A-7FCA-4428-B4E5-14004789C20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1560,6 +1560,53 @@
         <v>0</v>
       </c>
     </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>-1000</v>
+      </c>
+      <c r="H25">
+        <v>3000</v>
+      </c>
+      <c r="I25">
+        <v>-2000</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>98</v>
+      </c>
+      <c r="M25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>4140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated charging controller to allow charging both vehicles if immediate charging enabled
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62426A9A-7FCA-4428-B4E5-14004789C20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812CFDF4-802F-4D1E-811F-509765B8F1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -102,12 +102,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,8 +128,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -522,192 +529,192 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
         <v>-4500</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>4500</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>10</v>
       </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
         <v>-4500</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>4500</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
         <v>90</v>
       </c>
-      <c r="M4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4">
+      <c r="M4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
         <v>-9000</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>9000</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
         <v>10</v>
       </c>
-      <c r="M5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
+      <c r="M5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="1">
+        <v>0</v>
+      </c>
+      <c r="O5" s="1">
         <f>H5-3800</f>
         <v>5200</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
         <v>-4500</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>8000</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>-3500</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>10</v>
       </c>
-      <c r="M6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
+      <c r="M6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0</v>
+      </c>
+      <c r="O6" s="1">
         <f>H6-3800</f>
         <v>4200</v>
       </c>
@@ -947,476 +954,476 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>3</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
         <v>-100</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>100</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>90</v>
       </c>
-      <c r="M12" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="1">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>3</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
         <v>-2000</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>2000</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
         <v>10</v>
       </c>
-      <c r="M13" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="M13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="1">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>3</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
         <v>-2000</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>2000</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
         <v>50</v>
       </c>
-      <c r="M14" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14">
+      <c r="M14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
         <f>230*6*3</f>
         <v>4140</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>3</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
         <v>-4500</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="1">
         <v>4500</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
         <v>10</v>
       </c>
-      <c r="M15" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
+      <c r="M15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
         <v>4140</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
         <v>-4500</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="1">
         <v>4500</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
         <v>90</v>
       </c>
-      <c r="M16" t="s">
-        <v>9</v>
-      </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16">
+      <c r="M16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
         <v>4500</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
         <v>-4500</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="1">
         <v>8000</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>-3500</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
         <v>10</v>
       </c>
-      <c r="M17" t="s">
-        <v>9</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
+      <c r="M17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
         <f>8000-3800</f>
         <v>4200</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>3</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
         <v>-4500</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="1">
         <v>8000</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>-3500</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
         <v>50</v>
       </c>
-      <c r="M18" t="s">
-        <v>9</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
+      <c r="M18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
         <v>8000</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
         <v>1000</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="1">
         <v>3500</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
         <v>4500</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>50</v>
       </c>
-      <c r="M19" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
+      <c r="M19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
         <v>4140</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>5000</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>10</v>
-      </c>
-      <c r="M20" t="s">
-        <v>9</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1300</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>98</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
         <v>4140</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>5000</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>10</v>
-      </c>
-      <c r="M21" t="s">
-        <v>9</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>8000</v>
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-2000</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>98</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>4140</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
@@ -1424,7 +1431,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1439,13 +1446,13 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H22">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1454,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="M22" t="s">
         <v>9</v>
@@ -1471,7 +1478,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1480,16 +1487,16 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>-9000</v>
+        <v>5000</v>
       </c>
       <c r="H23">
-        <v>9000</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1501,16 +1508,16 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="M23" t="s">
         <v>9</v>
       </c>
       <c r="N23">
-        <v>0</v>
+        <v>4140</v>
       </c>
       <c r="O23">
-        <v>0</v>
+        <v>4140</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
@@ -1560,54 +1567,104 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>3</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>-1000</v>
-      </c>
-      <c r="H25">
-        <v>3000</v>
-      </c>
-      <c r="I25">
-        <v>-2000</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
+      <c r="B25" s="1">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>10</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>-9000</v>
+      </c>
+      <c r="H26" s="1">
+        <v>9000</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
         <v>98</v>
       </c>
-      <c r="M25" t="s">
-        <v>16</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>4140</v>
+      <c r="M26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O26">
+    <sortCondition ref="B2:B26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed charging logic for Level 1
</commit_message>
<xml_diff>
--- a/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
+++ b/ChargingController/ChargingControllerTests/TestCases/ChargingDecisions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\GitHub\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThomasSchissler\source\repos\github\tschissler\SmartHomeTS\ChargingController\ChargingControllerTests\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812CFDF4-802F-4D1E-811F-509765B8F1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB0FFFD-A584-49E1-BBEB-0288EDCDB3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53800" yWindow="630" windowWidth="25620" windowHeight="21770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>InsideConnected</t>
   </si>
@@ -411,31 +411,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -517,7 +517,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M2" t="s">
         <v>9</v>
@@ -529,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -573,10 +573,10 @@
         <v>0</v>
       </c>
       <c r="O3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -596,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>-4500</v>
+        <v>-2000</v>
       </c>
       <c r="H4" s="1">
         <v>4500</v>
@@ -620,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -643,10 +643,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>-9000</v>
+        <v>-3900</v>
       </c>
       <c r="H5" s="1">
-        <v>9000</v>
+        <v>4500</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
@@ -667,11 +667,10 @@
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <f>H5-3800</f>
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -715,58 +714,57 @@
         <v>0</v>
       </c>
       <c r="O6" s="1">
-        <f>H6-3800</f>
         <v>4200</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>-2000</v>
-      </c>
-      <c r="H7">
-        <v>2000</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>10</v>
-      </c>
-      <c r="M7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-3000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>6000</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-3000</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>95</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+      <c r="O7" s="1">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -786,10 +784,10 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>-4500</v>
+        <v>-2000</v>
       </c>
       <c r="H8">
-        <v>4500</v>
+        <v>2000</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -810,10 +808,10 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -848,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="M9" t="s">
         <v>9</v>
@@ -860,7 +858,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -880,10 +878,10 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>-9000</v>
+        <v>-4500</v>
       </c>
       <c r="H10">
-        <v>9000</v>
+        <v>4500</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -895,7 +893,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="M10" t="s">
         <v>9</v>
@@ -904,10 +902,10 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -927,13 +925,13 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>-4500</v>
+        <v>-9000</v>
       </c>
       <c r="H11">
-        <v>8000</v>
+        <v>9000</v>
       </c>
       <c r="I11">
-        <v>-3500</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -951,57 +949,57 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
-        <v>3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>-100</v>
-      </c>
-      <c r="H12" s="1">
-        <v>100</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <v>90</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>-4500</v>
+      </c>
+      <c r="H12">
+        <v>8000</v>
+      </c>
+      <c r="I12">
+        <v>-3500</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>10</v>
+      </c>
+      <c r="M12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1021,10 +1019,10 @@
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>-2000</v>
+        <v>-100</v>
       </c>
       <c r="H13" s="1">
-        <v>2000</v>
+        <v>100</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -1036,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="1">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>9</v>
@@ -1048,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1083,67 +1081,67 @@
         <v>0</v>
       </c>
       <c r="L14" s="1">
+        <v>10</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-2000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
         <v>50</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1">
+      <c r="M15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
         <f>230*6*3</f>
         <v>4140</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>3</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>-4500</v>
-      </c>
-      <c r="H15" s="1">
-        <v>4500</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>10</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>4140</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1178,7 +1176,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>9</v>
@@ -1187,10 +1185,10 @@
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1213,79 +1211,79 @@
         <v>-4500</v>
       </c>
       <c r="H17" s="1">
+        <v>4500</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>90</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>-4500</v>
+      </c>
+      <c r="H18" s="1">
         <v>8000</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I18" s="1">
         <v>-3500</v>
       </c>
-      <c r="J17" s="1">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
         <v>10</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N17" s="1">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1">
+      <c r="M18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
         <f>8000-3800</f>
         <v>4200</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>3</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1">
-        <v>-4500</v>
-      </c>
-      <c r="H18" s="1">
-        <v>8000</v>
-      </c>
-      <c r="I18" s="1">
-        <v>-3500</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1">
-        <v>50</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N18" s="1">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1305,19 +1303,19 @@
         <v>1</v>
       </c>
       <c r="G19" s="1">
-        <v>0</v>
+        <v>-4500</v>
       </c>
       <c r="H19" s="1">
-        <v>1000</v>
+        <v>8000</v>
       </c>
       <c r="I19" s="1">
-        <v>3500</v>
+        <v>-3500</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
       </c>
       <c r="K19" s="1">
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="L19" s="1">
         <v>50</v>
@@ -1329,10 +1327,10 @@
         <v>0</v>
       </c>
       <c r="O19" s="1">
-        <v>4140</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1355,19 +1353,19 @@
         <v>0</v>
       </c>
       <c r="H20" s="1">
-        <v>1300</v>
+        <v>1000</v>
       </c>
       <c r="I20" s="1">
-        <v>-1000</v>
+        <v>3500</v>
       </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
       <c r="K20" s="1">
-        <v>0</v>
+        <v>4500</v>
       </c>
       <c r="L20" s="1">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>9</v>
@@ -1379,7 +1377,7 @@
         <v>4140</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1399,13 +1397,13 @@
         <v>1</v>
       </c>
       <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1300</v>
+      </c>
+      <c r="I21" s="1">
         <v>-1000</v>
-      </c>
-      <c r="H21" s="1">
-        <v>3000</v>
-      </c>
-      <c r="I21" s="1">
-        <v>-2000</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
@@ -1417,7 +1415,7 @@
         <v>98</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
@@ -1426,54 +1424,54 @@
         <v>4140</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
-        <v>5000</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>10</v>
-      </c>
-      <c r="M22" t="s">
-        <v>9</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>-1000</v>
+      </c>
+      <c r="H22" s="1">
+        <v>3000</v>
+      </c>
+      <c r="I22" s="1">
+        <v>-2000</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>98</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
         <v>4140</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1481,7 +1479,7 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1514,13 +1512,13 @@
         <v>9</v>
       </c>
       <c r="N23">
-        <v>4140</v>
+        <v>0</v>
       </c>
       <c r="O23">
         <v>4140</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1528,19 +1526,19 @@
         <v>4</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1555,66 +1553,66 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="M24" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>4140</v>
       </c>
       <c r="O24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1">
-        <v>5000</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0</v>
-      </c>
-      <c r="I25" s="1">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1">
-        <v>0</v>
-      </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1">
-        <v>10</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N25" s="1">
-        <v>0</v>
-      </c>
-      <c r="O25" s="1">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>98</v>
+      </c>
+      <c r="M25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1622,48 +1620,95 @@
         <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26" s="1">
+        <v>5000</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>10</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="1">
+        <v>0</v>
+      </c>
+      <c r="O26" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
         <v>-9000</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H27" s="1">
         <v>9000</v>
       </c>
-      <c r="I26" s="1">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1">
-        <v>0</v>
-      </c>
-      <c r="K26" s="1">
-        <v>0</v>
-      </c>
-      <c r="L26" s="1">
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
         <v>98</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N26" s="1">
-        <v>0</v>
-      </c>
-      <c r="O26" s="1">
+      <c r="M27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O26">
-    <sortCondition ref="B2:B26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O27">
+    <sortCondition ref="B2:B27"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>